<commit_message>
File changes and update
</commit_message>
<xml_diff>
--- a/munka_menet_utemterv.xlsx
+++ b/munka_menet_utemterv.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB440BF1-2E1A-402B-872A-61B8C91CD278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB5E005-6272-4B0D-BB82-70D62973D0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1435,7 +1435,7 @@
       <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="H2" s="9">
         <f ca="1">TODAY()-(L1-1)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J2" s="17"/>
       <c r="K2" s="38" t="s">
@@ -2746,13 +2746,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="18">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E7" s="18">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F7" s="18">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G7" s="28">
         <v>0</v>

</xml_diff>